<commit_message>
Atualizando referencias erradas no documento
</commit_message>
<xml_diff>
--- a/Processo/Avaliação/GPR-Avaliação Projeto.xlsx
+++ b/Processo/Avaliação/GPR-Avaliação Projeto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="57">
   <si>
     <t>Gerência de Projetos</t>
   </si>
@@ -179,9 +179,6 @@
 As evidências apresentadas para este resultado permitem assegurar: (i) que foi definida uma política organizacional estabelecendo as expectativas da organização para a execução do processo e que esta política é conhecida e de fácil acesso aos interessados? (ii) que a política organizacional foi atualizada, quando necessário? (iii) que a política organizacional tem respaldo da alta administração (por exemplo, por meio de aprovação da alta administração)?</t>
   </si>
   <si>
-    <t>Plano de projeto</t>
-  </si>
-  <si>
     <t xml:space="preserve">RAP 3. A execução do processo é planejada.
 As evidências apresentadas para este resultado permitem assegurar que existe um plano para a execução do processo?                                                   </t>
   </si>
@@ -198,9 +195,6 @@
 As evidências apresentadas para este resultado permitem assegurar que foi fornecido treinamento  formal (cursos) ou informal (mentoring) para a execução do processo? (Considerar que, quando o indivíduo já possui o perfil e habilidades para executar o processo, o treinamento é dispensável.)</t>
   </si>
   <si>
-    <t>Documento de Definição de Processo de Gerência de Projeto</t>
-  </si>
-  <si>
     <t>RAP 8. A comunicação entre as partes interessadas no processo é planejada e executada de forma a garantir o seu envolvimento.
 As evidências apresentadas para este resultado permitem assegurar que: (i) foi planejada a comunicação entre as partes interessadas no processo?; (ii) este planejamento foi monitorado?; (iii) existe evidência de que a comunicação ocorre de forma a garantir o envolvimento das partes interessadas?</t>
   </si>
@@ -209,14 +203,23 @@
 As evidências apresentadas para este resultado permitem assegurar que o projeto foi conduzido a partir da execução do seu processo planejado, bem como se existem registros de execução das atividades do processo com base no seu planejamento?</t>
   </si>
   <si>
-    <t>Documento de Acompanhamento de Não-Conformidades</t>
+    <t>Relatório de Não-Conformidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plano de Gerencia de Projeto </t>
+  </si>
+  <si>
+    <t>Documento de Definição de Processo de Gerência de Projeto (Item 6 comunicação )</t>
+  </si>
+  <si>
+    <t>Documento de Definição de Processo de Gerência de Projeto ( Item 4 )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -269,11 +272,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0066CC"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -306,13 +304,12 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -603,7 +600,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -691,59 +688,59 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -29069,8 +29066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29244,7 +29241,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="46" t="str">
+      <c r="C6" s="45" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -29449,7 +29446,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21"/>
-      <c r="C13" s="45" t="str">
+      <c r="C13" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -29654,7 +29651,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="C20" s="45" t="str">
+      <c r="C20" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento do Or%C3%A7amento.docx","X")</f>
         <v>X</v>
       </c>
@@ -29859,7 +29856,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="21"/>
-      <c r="C27" s="45" t="str">
+      <c r="C27" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento do Or%C3%A7amento.docx","X")</f>
         <v>X</v>
       </c>
@@ -29892,7 +29889,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="21"/>
-      <c r="C28" s="45" t="str">
+      <c r="C28" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciamento%20do%20Cronograma.docx","X")</f>
         <v>X</v>
       </c>
@@ -29925,10 +29922,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="21"/>
-      <c r="C29" s="25" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C29" s="44"/>
       <c r="D29" s="21"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -30074,7 +30068,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="21"/>
-      <c r="C34" s="45" t="str">
+      <c r="C34" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciade%20de%20Riscos.docx","X")</f>
         <v>X</v>
       </c>
@@ -30279,7 +30273,7 @@
         <v>30</v>
       </c>
       <c r="B41" s="21"/>
-      <c r="C41" s="45" t="str">
+      <c r="C41" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
         <v>X</v>
       </c>
@@ -30312,7 +30306,7 @@
         <v>31</v>
       </c>
       <c r="B42" s="21"/>
-      <c r="C42" s="45" t="str">
+      <c r="C42" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
         <v>X</v>
       </c>
@@ -30486,11 +30480,11 @@
     </row>
     <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B48" s="21"/>
-      <c r="C48" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
+      <c r="C48" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento do Or%C3%A7amento.docx","X")</f>
         <v>X</v>
       </c>
       <c r="D48" s="21"/>
@@ -30518,9 +30512,14 @@
       <c r="Z48" s="5"/>
     </row>
     <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="20"/>
+      <c r="A49" s="46" t="s">
+        <v>35</v>
+      </c>
       <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
+      <c r="C49" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx","X")</f>
+        <v>X</v>
+      </c>
       <c r="D49" s="21"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -30694,7 +30693,7 @@
         <v>11</v>
       </c>
       <c r="B55" s="21"/>
-      <c r="C55" s="45" t="str">
+      <c r="C55" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -30723,9 +30722,14 @@
       <c r="Z55" s="5"/>
     </row>
     <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20"/>
+      <c r="A56" s="46" t="s">
+        <v>35</v>
+      </c>
       <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="C56" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx","X")</f>
+        <v>X</v>
+      </c>
       <c r="D56" s="21"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -30895,11 +30899,11 @@
       <c r="Z61" s="5"/>
     </row>
     <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="48" t="s">
+      <c r="A62" s="46" t="s">
         <v>35</v>
       </c>
       <c r="B62" s="21"/>
-      <c r="C62" s="25" t="str">
+      <c r="C62" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx","X")</f>
         <v>X</v>
       </c>
@@ -31104,7 +31108,7 @@
         <v>37</v>
       </c>
       <c r="B69" s="21"/>
-      <c r="C69" s="31" t="str">
+      <c r="C69" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/GPR-Ger%C3%AAncia%20de%20Projeto.docx.docx","X")</f>
         <v>X</v>
       </c>
@@ -31309,7 +31313,7 @@
         <v>11</v>
       </c>
       <c r="B76" s="21"/>
-      <c r="C76" s="45" t="str">
+      <c r="C76" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -31342,7 +31346,7 @@
         <v>23</v>
       </c>
       <c r="B77" s="21"/>
-      <c r="C77" s="45" t="str">
+      <c r="C77" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento do Or%C3%A7amento.docx","X")</f>
         <v>X</v>
       </c>
@@ -31375,7 +31379,7 @@
         <v>25</v>
       </c>
       <c r="B78" s="21"/>
-      <c r="C78" s="45" t="str">
+      <c r="C78" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciamento%20do%20Cronograma.docx","X")</f>
         <v>X</v>
       </c>
@@ -31408,10 +31412,7 @@
         <v>26</v>
       </c>
       <c r="B79" s="21"/>
-      <c r="C79" s="25" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C79" s="25"/>
       <c r="D79" s="21"/>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -31529,7 +31530,7 @@
         <v>11</v>
       </c>
       <c r="B83" s="21"/>
-      <c r="C83" s="45" t="str">
+      <c r="C83" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -31700,7 +31701,7 @@
       <c r="Z88" s="5"/>
     </row>
     <row r="89" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="32" t="s">
+      <c r="A89" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B89" s="13"/>
@@ -31734,10 +31735,7 @@
         <v>37</v>
       </c>
       <c r="B90" s="21"/>
-      <c r="C90" s="31" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/GPR-Ger%C3%AAncia%20de%20Projeto.docx.docx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C90" s="44"/>
       <c r="D90" s="21"/>
       <c r="E90" s="5"/>
       <c r="F90" s="5"/>
@@ -31767,10 +31765,7 @@
         <v>26</v>
       </c>
       <c r="B91" s="21"/>
-      <c r="C91" s="25" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C91" s="25"/>
       <c r="D91" s="21"/>
       <c r="E91" s="5"/>
       <c r="F91" s="5"/>
@@ -31800,10 +31795,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="21"/>
-      <c r="C92" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciade%20de%20Riscos.docx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C92" s="44"/>
       <c r="D92" s="21"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
@@ -31915,7 +31907,7 @@
       <c r="Z95" s="5"/>
     </row>
     <row r="96" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="32" t="s">
+      <c r="A96" s="31" t="s">
         <v>41</v>
       </c>
       <c r="B96" s="13"/>
@@ -31949,10 +31941,7 @@
         <v>35</v>
       </c>
       <c r="B97" s="21"/>
-      <c r="C97" s="25" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C97" s="44"/>
       <c r="D97" s="21"/>
       <c r="E97" s="5"/>
       <c r="F97" s="5"/>
@@ -31982,10 +31971,7 @@
         <v>30</v>
       </c>
       <c r="B98" s="21"/>
-      <c r="C98" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C98" s="44"/>
       <c r="D98" s="21"/>
       <c r="E98" s="5"/>
       <c r="F98" s="5"/>
@@ -32015,10 +32001,7 @@
         <v>31</v>
       </c>
       <c r="B99" s="21"/>
-      <c r="C99" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C99" s="44"/>
       <c r="D99" s="21"/>
       <c r="E99" s="5"/>
       <c r="F99" s="5"/>
@@ -32130,7 +32113,7 @@
       <c r="Z102" s="5"/>
     </row>
     <row r="103" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="32" t="s">
+      <c r="A103" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B103" s="13"/>
@@ -32164,10 +32147,7 @@
         <v>43</v>
       </c>
       <c r="B104" s="21"/>
-      <c r="C104" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciade%20de%20Riscos.docx","X")</f>
-        <v>X</v>
-      </c>
+      <c r="C104" s="44"/>
       <c r="D104" s="21"/>
       <c r="E104" s="5"/>
       <c r="F104" s="5"/>
@@ -32197,7 +32177,7 @@
         <v>28</v>
       </c>
       <c r="B105" s="21"/>
-      <c r="C105" s="45" t="str">
+      <c r="C105" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciade%20de%20Riscos.docx","X")</f>
         <v>X</v>
       </c>
@@ -32340,12 +32320,12 @@
       <c r="Z109" s="5"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B110" s="34"/>
-      <c r="C110" s="34"/>
-      <c r="D110" s="34"/>
+      <c r="B110" s="33"/>
+      <c r="C110" s="33"/>
+      <c r="D110" s="33"/>
       <c r="E110" s="5"/>
       <c r="F110" s="5"/>
       <c r="G110" s="5"/>
@@ -32370,12 +32350,12 @@
       <c r="Z110" s="5"/>
     </row>
     <row r="111" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="35" t="s">
+      <c r="A111" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B111" s="36"/>
-      <c r="C111" s="36"/>
-      <c r="D111" s="36"/>
+      <c r="B111" s="35"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="35"/>
       <c r="E111" s="5"/>
       <c r="F111" s="5"/>
       <c r="G111" s="5"/>
@@ -32400,12 +32380,12 @@
       <c r="Z111" s="5"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B112" s="38"/>
-      <c r="C112" s="39"/>
-      <c r="D112" s="39"/>
+      <c r="B112" s="37"/>
+      <c r="C112" s="38"/>
+      <c r="D112" s="38"/>
       <c r="E112" s="5"/>
       <c r="F112" s="5"/>
       <c r="G112" s="5"/>
@@ -32430,12 +32410,12 @@
       <c r="Z112" s="5"/>
     </row>
     <row r="113" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="40" t="s">
+      <c r="A113" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B113" s="41"/>
-      <c r="C113" s="42"/>
-      <c r="D113" s="42"/>
+      <c r="B113" s="40"/>
+      <c r="C113" s="41"/>
+      <c r="D113" s="41"/>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -32460,12 +32440,12 @@
       <c r="Z113" s="5"/>
     </row>
     <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="20" t="s">
-        <v>47</v>
+      <c r="A114" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="B114" s="21"/>
-      <c r="C114" s="45" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
+      <c r="C114" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/GPR-Ger%C3%AAncia%20de%20Projeto.docx.docx","X")</f>
         <v>X</v>
       </c>
       <c r="D114" s="21"/>
@@ -32635,12 +32615,12 @@
       <c r="Z119" s="5"/>
     </row>
     <row r="120" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="40" t="s">
-        <v>48</v>
+      <c r="A120" s="39" t="s">
+        <v>47</v>
       </c>
-      <c r="B120" s="43"/>
-      <c r="C120" s="44"/>
-      <c r="D120" s="44"/>
+      <c r="B120" s="42"/>
+      <c r="C120" s="43"/>
+      <c r="D120" s="43"/>
       <c r="E120" s="5"/>
       <c r="F120" s="5"/>
       <c r="G120" s="5"/>
@@ -32666,11 +32646,11 @@
     </row>
     <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B121" s="21"/>
-      <c r="C121" s="25" t="str">
-        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx","X")</f>
+      <c r="C121" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano%20de%20Gerenciamento%20do%20Cronograma.docx","X")</f>
         <v>X</v>
       </c>
       <c r="D121" s="21"/>
@@ -32698,9 +32678,14 @@
       <c r="Z121" s="5"/>
     </row>
     <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="20"/>
+      <c r="A122" s="20" t="s">
+        <v>11</v>
+      </c>
       <c r="B122" s="21"/>
-      <c r="C122" s="21"/>
+      <c r="C122" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
+        <v>X</v>
+      </c>
       <c r="D122" s="21"/>
       <c r="E122" s="5"/>
       <c r="F122" s="5"/>
@@ -32726,9 +32711,14 @@
       <c r="Z122" s="5"/>
     </row>
     <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="20"/>
+      <c r="A123" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="B123" s="21"/>
-      <c r="C123" s="21"/>
+      <c r="C123" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/GPR-Ger%C3%AAncia%20de%20Projeto.docx.docx","X")</f>
+        <v>X</v>
+      </c>
       <c r="D123" s="21"/>
       <c r="E123" s="5"/>
       <c r="F123" s="5"/>
@@ -32757,7 +32747,7 @@
       <c r="A124" s="20"/>
       <c r="B124" s="21"/>
       <c r="C124" s="21"/>
-      <c r="D124" s="21"/>
+      <c r="D124" s="48"/>
       <c r="E124" s="5"/>
       <c r="F124" s="5"/>
       <c r="G124" s="5"/>
@@ -32840,12 +32830,12 @@
       <c r="Z126" s="5"/>
     </row>
     <row r="127" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="40" t="s">
-        <v>49</v>
+      <c r="A127" s="39" t="s">
+        <v>48</v>
       </c>
-      <c r="B127" s="44"/>
-      <c r="C127" s="44"/>
-      <c r="D127" s="44"/>
+      <c r="B127" s="43"/>
+      <c r="C127" s="43"/>
+      <c r="D127" s="43"/>
       <c r="E127" s="5"/>
       <c r="F127" s="5"/>
       <c r="G127" s="5"/>
@@ -32874,7 +32864,7 @@
         <v>31</v>
       </c>
       <c r="B128" s="21"/>
-      <c r="C128" s="45" t="str">
+      <c r="C128" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
         <v>X</v>
       </c>
@@ -32907,7 +32897,7 @@
         <v>11</v>
       </c>
       <c r="B129" s="21"/>
-      <c r="C129" s="45" t="str">
+      <c r="C129" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano%20de%20Projeto.pdf","X")</f>
         <v>X</v>
       </c>
@@ -33050,12 +33040,12 @@
       <c r="Z133" s="5"/>
     </row>
     <row r="134" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="40" t="s">
-        <v>50</v>
+      <c r="A134" s="39" t="s">
+        <v>49</v>
       </c>
-      <c r="B134" s="44"/>
-      <c r="C134" s="44"/>
-      <c r="D134" s="44"/>
+      <c r="B134" s="43"/>
+      <c r="C134" s="43"/>
+      <c r="D134" s="43"/>
       <c r="E134" s="5"/>
       <c r="F134" s="5"/>
       <c r="G134" s="5"/>
@@ -33084,7 +33074,7 @@
         <v>31</v>
       </c>
       <c r="B135" s="21"/>
-      <c r="C135" s="47" t="str">
+      <c r="C135" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
         <v>X</v>
       </c>
@@ -33255,12 +33245,12 @@
       <c r="Z140" s="5"/>
     </row>
     <row r="141" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="40" t="s">
-        <v>51</v>
+      <c r="A141" s="39" t="s">
+        <v>50</v>
       </c>
-      <c r="B141" s="44"/>
-      <c r="C141" s="44"/>
-      <c r="D141" s="44"/>
+      <c r="B141" s="43"/>
+      <c r="C141" s="43"/>
+      <c r="D141" s="43"/>
       <c r="E141" s="5"/>
       <c r="F141" s="5"/>
       <c r="G141" s="5"/>
@@ -33285,11 +33275,11 @@
       <c r="Z141" s="5"/>
     </row>
     <row r="142" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="20" t="s">
-        <v>52</v>
+      <c r="A142" s="46" t="s">
+        <v>56</v>
       </c>
       <c r="B142" s="21"/>
-      <c r="C142" s="45" t="str">
+      <c r="C142" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx","X")</f>
         <v>X</v>
       </c>
@@ -33318,9 +33308,14 @@
       <c r="Z142" s="5"/>
     </row>
     <row r="143" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="20"/>
+      <c r="A143" s="20" t="s">
+        <v>31</v>
+      </c>
       <c r="B143" s="21"/>
-      <c r="C143" s="21"/>
+      <c r="C143" s="44" t="str">
+        <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates%20GPR/Plano de Gerência de Recursos Humanos.docx ","X")</f>
+        <v>X</v>
+      </c>
       <c r="D143" s="21"/>
       <c r="E143" s="5"/>
       <c r="F143" s="5"/>
@@ -33374,7 +33369,7 @@
       <c r="Z144" s="5"/>
     </row>
     <row r="145" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="20"/>
+      <c r="A145" s="47"/>
       <c r="B145" s="21"/>
       <c r="C145" s="21"/>
       <c r="D145" s="21"/>
@@ -33460,12 +33455,12 @@
       <c r="Z147" s="5"/>
     </row>
     <row r="148" spans="1:26" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="40" t="s">
-        <v>53</v>
+      <c r="A148" s="39" t="s">
+        <v>51</v>
       </c>
-      <c r="B148" s="44"/>
-      <c r="C148" s="44"/>
-      <c r="D148" s="44"/>
+      <c r="B148" s="43"/>
+      <c r="C148" s="43"/>
+      <c r="D148" s="43"/>
       <c r="E148" s="5"/>
       <c r="F148" s="5"/>
       <c r="G148" s="5"/>
@@ -33491,10 +33486,10 @@
     </row>
     <row r="149" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="20" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B149" s="21"/>
-      <c r="C149" s="45" t="str">
+      <c r="C149" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx","X")</f>
         <v>X</v>
       </c>
@@ -33579,7 +33574,7 @@
       <c r="Z151" s="5"/>
     </row>
     <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="20"/>
+      <c r="A152" s="47"/>
       <c r="B152" s="21"/>
       <c r="C152" s="21"/>
       <c r="D152" s="21"/>
@@ -33665,12 +33660,12 @@
       <c r="Z154" s="5"/>
     </row>
     <row r="155" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="40" t="s">
-        <v>54</v>
+      <c r="A155" s="39" t="s">
+        <v>52</v>
       </c>
-      <c r="B155" s="44"/>
-      <c r="C155" s="44"/>
-      <c r="D155" s="44"/>
+      <c r="B155" s="43"/>
+      <c r="C155" s="43"/>
+      <c r="D155" s="43"/>
       <c r="E155" s="5"/>
       <c r="F155" s="5"/>
       <c r="G155" s="5"/>
@@ -33696,10 +33691,10 @@
     </row>
     <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B156" s="21"/>
-      <c r="C156" s="25" t="str">
+      <c r="C156" s="44" t="str">
         <f>HYPERLINK("https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GQA/G5-VAL-Relat%C3%B3rio de N%C3%A3o Conformidade-Template.xls.xlsx","X")</f>
         <v>X</v>
       </c>
@@ -57366,39 +57361,35 @@
     <hyperlink ref="C6" r:id="rId1" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
     <hyperlink ref="C20" r:id="rId2" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
     <hyperlink ref="C28" r:id="rId3" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Cronograma.pdf"/>
-    <hyperlink ref="C29" r:id="rId4" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx"/>
-    <hyperlink ref="C34" r:id="rId5" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
-    <hyperlink ref="C41" r:id="rId6" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
-    <hyperlink ref="C62" r:id="rId7" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx"/>
-    <hyperlink ref="C69" r:id="rId8" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/GPR-Ger%C3%AAncia de Projeto.docx.docx"/>
-    <hyperlink ref="C79" r:id="rId9" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx"/>
-    <hyperlink ref="C90" r:id="rId10" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/GPR-Ger%C3%AAncia de Projeto.docx.docx"/>
-    <hyperlink ref="C91" r:id="rId11" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx"/>
-    <hyperlink ref="C97" r:id="rId12" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Gerenciamento de Dados.docx"/>
-    <hyperlink ref="C121" r:id="rId13" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GPR/Plano de Monitoramento do Cronograma.xlsx"/>
-    <hyperlink ref="C142" r:id="rId14" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
-    <hyperlink ref="C149" r:id="rId15" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
-    <hyperlink ref="C156" r:id="rId16" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Template/Templates GQA/G5-VAL-Relat%C3%B3rio de N%C3%A3o Conformidade-Template.xls.xlsx"/>
-    <hyperlink ref="C13" r:id="rId17" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C48" r:id="rId18" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C55" r:id="rId19" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C76" r:id="rId20" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C83" r:id="rId21" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C114" r:id="rId22" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C129" r:id="rId23" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
-    <hyperlink ref="C27" r:id="rId24" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
-    <hyperlink ref="C77" r:id="rId25" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
-    <hyperlink ref="C78" r:id="rId26" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Cronograma.pdf"/>
-    <hyperlink ref="C92" r:id="rId27" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
-    <hyperlink ref="C105" r:id="rId28" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
-    <hyperlink ref="C98" r:id="rId29" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
-    <hyperlink ref="C99" r:id="rId30" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
-    <hyperlink ref="C104" r:id="rId31" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
-    <hyperlink ref="C128" r:id="rId32" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
-    <hyperlink ref="C135" r:id="rId33" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
-    <hyperlink ref="C42" r:id="rId34" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
+    <hyperlink ref="C34" r:id="rId4" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
+    <hyperlink ref="C41" r:id="rId5" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
+    <hyperlink ref="C62" r:id="rId6" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PGD_Plano de Gerenciamento de Dados.pdf"/>
+    <hyperlink ref="C69" r:id="rId7" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
+    <hyperlink ref="C142" r:id="rId8" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
+    <hyperlink ref="C149" r:id="rId9" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
+    <hyperlink ref="C13" r:id="rId10" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C55" r:id="rId11" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C76" r:id="rId12" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C83" r:id="rId13" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C129" r:id="rId14" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C77" r:id="rId15" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
+    <hyperlink ref="C78" r:id="rId16" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Cronograma.pdf"/>
+    <hyperlink ref="C105" r:id="rId17" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerencia dede Riscos.pdf"/>
+    <hyperlink ref="C128" r:id="rId18" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Ger%C3%AAncia de Recursos Humanos.pdf"/>
+    <hyperlink ref="C42" r:id="rId19" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PRH_Plano de Recursos Humanos.pdf"/>
+    <hyperlink ref="C27" r:id="rId20" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
+    <hyperlink ref="C48" r:id="rId21" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Or%C3%A7amento.pdf"/>
+    <hyperlink ref="C114" r:id="rId22" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
+    <hyperlink ref="C121" r:id="rId23" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Gerenciamento do Cronograma.pdf"/>
+    <hyperlink ref="C122" r:id="rId24" display="https://github.com/jeanlks/processoDeSoftware/blob/3768523d36c6855d14657fd4eaec7470e9d649fe/Projeto/GPR/Plano de Projeto.pdf"/>
+    <hyperlink ref="C156" r:id="rId25" display="https://github.com/jeanlks/processoDeSoftware/tree/master/Projeto/GQA/Relat%C3%B3rios de N%C3%A3o conformidade"/>
+    <hyperlink ref="C135" r:id="rId26" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PRH_Plano de Recursos Humanos.pdf"/>
+    <hyperlink ref="C143" r:id="rId27" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PRH_Plano de Recursos Humanos.pdf"/>
+    <hyperlink ref="C49" r:id="rId28" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PGD_Plano de Gerenciamento de Dados.pdf"/>
+    <hyperlink ref="C56" r:id="rId29" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Projeto/GPR/SGP_PGD_Plano de Gerenciamento de Dados.pdf"/>
+    <hyperlink ref="C123" r:id="rId30" display="https://github.com/jeanlks/processoDeSoftware/blob/master/Processo/Defini%C3%A7%C3%A3o/GPR-Processo.docx"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>